<commit_message>
final dmn table integrated
</commit_message>
<xml_diff>
--- a/documentation/bugs matterhorn.xlsx
+++ b/documentation/bugs matterhorn.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manuel.Frieder\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\digibp-matterhorn\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{33C39757-66CE-4DBF-B5BE-9695DE896C7C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17625" xr2:uid="{2C4F47FB-9F57-4C56-A7BC-28E1643F8904}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17625"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Task name</t>
   </si>
@@ -34,12 +33,21 @@
   </si>
   <si>
     <t>solved?</t>
+  </si>
+  <si>
+    <t>Evaluate the incident and find a solution</t>
+  </si>
+  <si>
+    <t>Solution field is not defined</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -385,11 +393,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A8C9188-12D0-4E04-A76F-458CC11806A4}">
-  <dimension ref="A1:C1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -409,6 +417,17 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>